<commit_message>
add some plots and indidivual analyses for species production vs aquauculture  effort
</commit_message>
<xml_diff>
--- a/Data/mari_area_fish_province.xlsx
+++ b/Data/mari_area_fish_province.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22188" windowHeight="8592" firstSheet="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22188" windowHeight="8592" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="37" r:id="rId1"/>
@@ -4132,8 +4132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4524,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4995,8 +4995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5466,8 +5466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5934,8 +5934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6399,8 +6399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6654,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6909,8 +6909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7164,8 +7164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7422,8 +7422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7677,8 +7677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7952,8 +7952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8345,8 +8345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8614,8 +8614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8850,8 +8850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9284,8 +9284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9520,8 +9520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10045,8 +10045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10476,8 +10476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11001,8 +11001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11432,8 +11432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11974,8 +11974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12380,8 +12380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12776,8 +12776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13193,8 +13193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13412,8 +13412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13614,8 +13614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14141,8 +14141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14164,8 +14164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14512,8 +14512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14770,8 +14770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15028,8 +15028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15424,8 +15424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15818,7 +15818,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15927,7 +15927,7 @@
         <v>763101</v>
       </c>
       <c r="C4">
-        <v>7.0750000000000002</v>
+        <v>7075</v>
       </c>
       <c r="D4" s="1">
         <v>19624</v>
@@ -16219,8 +16219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16625,8 +16625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17062,8 +17062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>